<commit_message>
Making a project plan document with 4 assigned tasks.
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,9 +13,173 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+  <si>
+    <t>LED Stringn Animation Project Plan  [PO5_LSAN]</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Discription</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Assignation Date</t>
+  </si>
+  <si>
+    <t>Estimated Time</t>
+  </si>
+  <si>
+    <t>Actual Delivery Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>Estimate Date</t>
+  </si>
+  <si>
+    <t>Make Template to the CYRS document</t>
+  </si>
+  <si>
+    <t>TASK001</t>
+  </si>
+  <si>
+    <t>Menna</t>
+  </si>
+  <si>
+    <t>Week1</t>
+  </si>
+  <si>
+    <t>Week2</t>
+  </si>
+  <si>
+    <t>Week3</t>
+  </si>
+  <si>
+    <t>Week4</t>
+  </si>
+  <si>
+    <t>Week5</t>
+  </si>
+  <si>
+    <t>Week6</t>
+  </si>
+  <si>
+    <t>Week7</t>
+  </si>
+  <si>
+    <t>Make Template to the SRS document</t>
+  </si>
+  <si>
+    <t>TASK002</t>
+  </si>
+  <si>
+    <t>Mohanad</t>
+  </si>
+  <si>
+    <t>Make Template to the HIS document</t>
+  </si>
+  <si>
+    <t>TASK003</t>
+  </si>
+  <si>
+    <t>TASK004</t>
+  </si>
+  <si>
+    <t>TASK005</t>
+  </si>
+  <si>
+    <t>TASK006</t>
+  </si>
+  <si>
+    <t>TASK007</t>
+  </si>
+  <si>
+    <t>TASK008</t>
+  </si>
+  <si>
+    <t>TASK009</t>
+  </si>
+  <si>
+    <t>TASK010</t>
+  </si>
+  <si>
+    <t>TASK011</t>
+  </si>
+  <si>
+    <t>TASK012</t>
+  </si>
+  <si>
+    <t>TASK013</t>
+  </si>
+  <si>
+    <t>TASK014</t>
+  </si>
+  <si>
+    <t>TASK015</t>
+  </si>
+  <si>
+    <t>Waleed</t>
+  </si>
+  <si>
+    <t>Make Template to the SIQ document</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>CYRS_TASK001_V1</t>
+  </si>
+  <si>
+    <t>TASK016</t>
+  </si>
+  <si>
+    <t>TASK017</t>
+  </si>
+  <si>
+    <t>TASK018</t>
+  </si>
+  <si>
+    <t>TASK019</t>
+  </si>
+  <si>
+    <t>SRS_TASK002_V1</t>
+  </si>
+  <si>
+    <t>HIS_TASK003_V1</t>
+  </si>
+  <si>
+    <t>SIQ_TASK004_V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asseigned </t>
+  </si>
+  <si>
+    <t>Members:</t>
+  </si>
+  <si>
+    <t>Team Lead: Youssef Kamal</t>
+  </si>
+  <si>
+    <t>Estimate Time</t>
+  </si>
+  <si>
+    <t>Waleed Adel - Sara Abd ElRahman - Mennatullah Mostafa - Mohanad Sallam</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +187,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -40,18 +245,237 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +522,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +557,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +765,606 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="13">
+        <v>43851</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="23"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="18">
+        <v>43851</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="25"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="18">
+        <v>43851</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="19"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="25"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="18">
+        <v>43851</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="25"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="25"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="25"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="25"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="25"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="25"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="25"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="25"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="25"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="25"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="25"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="25"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="25"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="25"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="25"/>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:S3"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J23">
+      <formula1>"Asseigned , In progress , done , Revised"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates HSI TASK Status
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -106,9 +106,6 @@
     <t>Mohanad</t>
   </si>
   <si>
-    <t>HIS_TASK003_V1</t>
-  </si>
-  <si>
     <t>TASK003</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>24h</t>
+  </si>
+  <si>
+    <t>HSI_TASK003_V1</t>
   </si>
 </sst>
 </file>
@@ -499,16 +499,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -526,6 +516,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -743,7 +743,7 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -762,77 +762,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="29" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="29" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
       <c r="T1" s="1"/>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
       <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -901,13 +901,13 @@
       <c r="D5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="25">
         <v>43851</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
       <c r="J5" s="11" t="s">
         <v>25</v>
       </c>
@@ -932,7 +932,7 @@
       <c r="D6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="26">
         <v>43851</v>
       </c>
       <c r="F6" s="1"/>
@@ -952,32 +952,32 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="D7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="26">
+        <v>43851</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="32">
-        <v>43851</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="34" t="s">
+      <c r="H7" s="28" t="s">
         <v>56</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>57</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K7" s="17"/>
       <c r="L7" s="15"/>
@@ -989,32 +989,32 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="C8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="E8" s="26">
+        <v>43851</v>
+      </c>
+      <c r="F8" s="29">
+        <v>43852</v>
+      </c>
+      <c r="G8" s="29">
+        <v>43854</v>
+      </c>
+      <c r="H8" s="30" t="s">
         <v>36</v>
-      </c>
-      <c r="E8" s="32">
-        <v>43851</v>
-      </c>
-      <c r="F8" s="35">
-        <v>43852</v>
-      </c>
-      <c r="G8" s="35">
-        <v>43854</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>37</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K8" s="17"/>
       <c r="L8" s="15"/>
@@ -1028,7 +1028,7 @@
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -1049,7 +1049,7 @@
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -1070,7 +1070,7 @@
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -1091,7 +1091,7 @@
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -1112,7 +1112,7 @@
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -1133,7 +1133,7 @@
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -1154,7 +1154,7 @@
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -1175,7 +1175,7 @@
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -1196,7 +1196,7 @@
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -1217,7 +1217,7 @@
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
@@ -1238,7 +1238,7 @@
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -1259,7 +1259,7 @@
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -1280,7 +1280,7 @@
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -1301,7 +1301,7 @@
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
@@ -1322,7 +1322,7 @@
       <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>

</xml_diff>

<commit_message>
Starting the SRS draft
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toshiba\Downloads\ITI\SW Engineering\SWProject\SW deliveries log\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>LED Stringn Animation Project Plan  [PO5_LSAN]</t>
   </si>
@@ -188,6 +193,9 @@
   </si>
   <si>
     <t>HSI_TASK003_V1</t>
+  </si>
+  <si>
+    <t>23/01/2020</t>
   </si>
 </sst>
 </file>
@@ -537,6 +545,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -743,7 +754,7 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -935,12 +946,18 @@
       <c r="E6" s="26">
         <v>43851</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>56</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="16" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="K6" s="17"/>
       <c r="L6" s="15"/>

</xml_diff>

<commit_message>
recieve Task : CYRS_TASK001_V1
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toshiba\Downloads\ITI\SW Engineering\SWProject\SW deliveries log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI_intake40\software_engineer\SW_Team_LEDString\master\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>LED Stringn Animation Project Plan  [PO5_LSAN]</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Menna</t>
   </si>
   <si>
-    <t xml:space="preserve">Asseigned </t>
-  </si>
-  <si>
     <t>SRS_TASK002_V1</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>23/01/2020</t>
+  </si>
+  <si>
+    <t>1h</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -534,6 +534,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -753,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -915,12 +918,18 @@
       <c r="E5" s="25">
         <v>43851</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="F5" s="37">
+        <v>43853</v>
+      </c>
+      <c r="G5" s="37">
+        <v>43853</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>58</v>
+      </c>
       <c r="I5" s="27"/>
       <c r="J5" s="11" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="K5" s="12"/>
       <c r="L5" s="10"/>
@@ -932,32 +941,32 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="C6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>29</v>
       </c>
       <c r="E6" s="26">
         <v>43851</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K6" s="17"/>
       <c r="L6" s="15"/>
@@ -969,32 +978,32 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>31</v>
       </c>
       <c r="E7" s="26">
         <v>43851</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="28" t="s">
         <v>55</v>
-      </c>
-      <c r="H7" s="28" t="s">
-        <v>56</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K7" s="17"/>
       <c r="L7" s="15"/>
@@ -1006,16 +1015,16 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="C8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="15" t="s">
         <v>34</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>35</v>
       </c>
       <c r="E8" s="26">
         <v>43851</v>
@@ -1027,11 +1036,11 @@
         <v>43854</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K8" s="17"/>
       <c r="L8" s="15"/>
@@ -1045,7 +1054,7 @@
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -1066,7 +1075,7 @@
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -1087,7 +1096,7 @@
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -1108,7 +1117,7 @@
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -1129,7 +1138,7 @@
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -1150,7 +1159,7 @@
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -1171,7 +1180,7 @@
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -1192,7 +1201,7 @@
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -1213,7 +1222,7 @@
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -1234,7 +1243,7 @@
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
@@ -1255,7 +1264,7 @@
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -1276,7 +1285,7 @@
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -1297,7 +1306,7 @@
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -1318,7 +1327,7 @@
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
@@ -1339,7 +1348,7 @@
       <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>

</xml_diff>

<commit_message>
Done with CYES Document
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>LED Stringn Animation Project Plan  [PO5_LSAN]</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>1h</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -526,6 +529,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -534,9 +540,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -776,77 +779,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="36" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="36" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
       <c r="T1" s="1"/>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
       <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -918,18 +921,20 @@
       <c r="E5" s="25">
         <v>43851</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="31">
         <v>43853</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="31">
         <v>43853</v>
       </c>
       <c r="H5" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="27"/>
+      <c r="I5" s="31">
+        <v>43853</v>
+      </c>
       <c r="J5" s="11" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K5" s="12"/>
       <c r="L5" s="10"/>

</xml_diff>

<commit_message>
-Update project plan task SIQ_TASK004_V1 from in progress to done
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SW engineering\SIQbranch\SW deliveries log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SW engineering\Master\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304D9815-7CAD-4138-A74E-2B7A2DC5A78A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F47F9E-6011-4264-ABF8-7072999CBD43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Team Lead: Youssef Kamal</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>LED String Animation Project Plan  [PO5_LSAN]</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -287,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -484,11 +487,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -547,6 +561,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1048,11 +1063,13 @@
       <c r="H8" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="J8" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="16"/>
+        <v>60</v>
+      </c>
+      <c r="K8" s="38"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>

</xml_diff>

<commit_message>
Creating Branches for the new TASKS
Creating New Branches for the new assigned tasks.
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>Team Lead: Youssef Kamal</t>
   </si>
@@ -220,6 +220,15 @@
   </si>
   <si>
     <t>Walid and Menna</t>
+  </si>
+  <si>
+    <t>REV_TO_CYRS_TASK007_V1</t>
+  </si>
+  <si>
+    <t>25/1/2020</t>
+  </si>
+  <si>
+    <t>Do the changes required in the review sheet to CYRS document</t>
   </si>
 </sst>
 </file>
@@ -281,7 +290,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +327,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -531,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -543,7 +558,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -594,6 +608,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,7 +619,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -969,58 +996,58 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>43851</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="28">
         <v>43853</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="28">
         <v>43853</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="12"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="11"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="23">
         <v>43851</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1029,435 +1056,445 @@
       <c r="G6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="25" t="s">
         <v>53</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="16"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="15"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="23">
         <v>43851</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="25" t="s">
         <v>53</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="16"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="15"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="23">
         <v>43851</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="26">
         <v>43852</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="26">
         <v>43854</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="27" t="s">
         <v>34</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="16"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="15"/>
     </row>
     <row r="9" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="15" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="K9" s="37"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="16"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="15"/>
     </row>
     <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="K10" s="37"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="16"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="15"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14" t="s">
+    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="16"/>
+      <c r="D11" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="15"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="16"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="15"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="16"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="15"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="16"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="15"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="16"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="15"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="16"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="15"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="16"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="15"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="16"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="15"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="16"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="15"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="16"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="15"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="16"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="15"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14" t="s">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="16"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="15"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="21"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="20"/>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updating actual start for TASK011
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SWE\PO5_LSAN\SW deliveries log\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
@@ -930,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1482,7 +1487,9 @@
       <c r="E15" s="34">
         <v>43892</v>
       </c>
-      <c r="F15" s="21"/>
+      <c r="F15" s="34">
+        <v>43892</v>
+      </c>
       <c r="G15" s="34">
         <v>43923</v>
       </c>
@@ -1550,22 +1557,18 @@
         <v>72</v>
       </c>
       <c r="E17" s="34">
-        <v>43892</v>
-      </c>
-      <c r="F17" s="34">
-        <v>43892</v>
-      </c>
+        <v>43923</v>
+      </c>
+      <c r="F17" s="34"/>
       <c r="G17" s="34">
-        <v>43923</v>
+        <v>43953</v>
       </c>
       <c r="H17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="34">
-        <v>43892</v>
-      </c>
+      <c r="I17" s="34"/>
       <c r="J17" s="30" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>

</xml_diff>

<commit_message>
Mohanad has done his task.
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SWE\PO5_LSAN\SW deliveries log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toshiba\Documents\GitHub\PO5_LSAN\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -282,9 +282,6 @@
     <t>Dead Line</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>SIQ_AKNOWLAGE_TASK015_V1</t>
   </si>
   <si>
@@ -304,12 +301,15 @@
   </si>
   <si>
     <t>48h</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -1010,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1158,7 +1158,7 @@
         <v>17</v>
       </c>
       <c r="R4" s="36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1520,7 +1520,7 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="38"/>
       <c r="R13" s="43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="75" x14ac:dyDescent="0.25">
@@ -1590,7 +1590,7 @@
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="22" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1622,7 +1622,7 @@
         <v>43984</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I16" s="13"/>
       <c r="J16" s="22" t="s">
@@ -1678,7 +1678,7 @@
         <v>83</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>42</v>
@@ -1711,10 +1711,10 @@
     </row>
     <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>43</v>
@@ -1732,7 +1732,7 @@
         <v>43923</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I19" s="26">
         <v>43923</v>

</xml_diff>

<commit_message>
Adding CDD for GPIO module
Adding CDD for GPIO module
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -1399,7 +1399,7 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2602,7 +2602,9 @@
       <c r="G33" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="H33" s="45"/>
+      <c r="H33" s="45">
+        <v>43892</v>
+      </c>
       <c r="I33" s="22" t="s">
         <v>53</v>
       </c>
@@ -2637,9 +2639,11 @@
       <c r="G34" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="H34" s="23"/>
+      <c r="H34" s="45">
+        <v>43896</v>
+      </c>
       <c r="I34" s="6" t="s">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="J34" s="23"/>
       <c r="K34" s="23"/>
@@ -2672,9 +2676,11 @@
       <c r="G35" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="H35" s="23"/>
+      <c r="H35" s="45">
+        <v>43896</v>
+      </c>
       <c r="I35" s="22" t="s">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="J35" s="23"/>
       <c r="K35" s="23"/>

</xml_diff>